<commit_message>
Cost mise en forme DBOM
</commit_message>
<xml_diff>
--- a/CR - Cost Report/CBOM/fasteners_processes_materials.xlsx
+++ b/CR - Cost Report/CBOM/fasteners_processes_materials.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fasteners!$A$1:$C$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Materials!$A$1:$C$84</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Processes!$A$1:$C$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Processes!$A$1:$C$43</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="151">
   <si>
     <t>Operation</t>
   </si>
@@ -135,27 +135,12 @@
     <t>Add with Ratchet for self-locking nuts</t>
   </si>
   <si>
-    <t>Micrometre</t>
-  </si>
-  <si>
     <t>Metrology</t>
   </si>
   <si>
-    <t>Inside micrometer</t>
-  </si>
-  <si>
     <t>Add for reamed holes</t>
   </si>
   <si>
-    <t>Indicator</t>
-  </si>
-  <si>
-    <t>Profile projector</t>
-  </si>
-  <si>
-    <t>Verification of reamed holes</t>
-  </si>
-  <si>
     <t>Use of lifting equipment (engine mainly)</t>
   </si>
   <si>
@@ -163,9 +148,6 @@
   </si>
   <si>
     <t>Before coating process, …</t>
-  </si>
-  <si>
-    <t>Verification for complexe machined parts, outside profiles</t>
   </si>
   <si>
     <t>Saw or tubing cut</t>
@@ -1720,11 +1702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,41 +1732,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1795,7 +1777,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1806,24 +1788,24 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1834,18 +1816,18 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1856,7 +1838,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1867,43 +1849,43 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,404 +1896,365 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
         <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
         <v>35</v>
-      </c>
-      <c r="C30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" t="s">
-        <v>155</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" t="s">
-        <v>153</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C46"/>
-  <conditionalFormatting sqref="D3 D29 C49:C54 C22:C47 D42 D36 C2:C20">
+  <autoFilter ref="A1:C43"/>
+  <conditionalFormatting sqref="D3 D27 C46:C51 D39 D33 C20:C44 C2:C18">
     <cfRule type="cellIs" dxfId="89" priority="3" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -2319,7 +2262,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -2328,7 +2271,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C43">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2342,7 +2285,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2354,7 +2297,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2368,222 +2311,222 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2682,8 +2625,8 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2695,7 +2638,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2709,444 +2652,444 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ca va être long
</commit_message>
<xml_diff>
--- a/CR - Cost Report/CBOM/fasteners_processes_materials.xlsx
+++ b/CR - Cost Report/CBOM/fasteners_processes_materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Processes" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fasteners!$A$1:$C$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Materials!$A$1:$C$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Materials!$A$1:$C$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Processes!$A$1:$C$43</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="152">
   <si>
     <t>Operation</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>First start, Engine</t>
+  </si>
+  <si>
+    <t>Seal, O-ring, Copper</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="92">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1704,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25:O25"/>
     </sheetView>
   </sheetViews>
@@ -2255,18 +2278,18 @@
   </sheetData>
   <autoFilter ref="A1:C43"/>
   <conditionalFormatting sqref="D3 D27 C46:C51 D39 D33 C20:C44 C2:C18">
-    <cfRule type="cellIs" dxfId="89" priority="3" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="3" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="4" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="1" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="2" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2285,7 +2308,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C18"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2532,82 +2555,82 @@
   </sheetData>
   <autoFilter ref="A1:C56"/>
   <conditionalFormatting sqref="C33:C64 D41 C14:D14 C17:C31 D18 C5:D6 C7:C11 D7:D10">
-    <cfRule type="cellIs" dxfId="85" priority="31" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="31" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="32" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="83" priority="29" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="29" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="30" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D4">
-    <cfRule type="cellIs" dxfId="81" priority="27" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="27" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="28" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="79" priority="21" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="21" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="22" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:D16">
-    <cfRule type="cellIs" dxfId="77" priority="19" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="19" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="20" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="75" priority="11" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="11" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="12" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="73" priority="7" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="7" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="8" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="71" priority="5" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="5" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="6" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="4" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="67" priority="1" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="2" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2622,11 +2645,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3016,10 +3039,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
         <v>49</v>
@@ -3027,21 +3050,18 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>49</v>
-      </c>
-      <c r="D32" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
         <v>106</v>
@@ -3055,7 +3075,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
         <v>106</v>
@@ -3069,10 +3089,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
         <v>49</v>
@@ -3083,18 +3103,40 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>90</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C84"/>
-  <conditionalFormatting sqref="C39:C42 C61:C92 D69 C43:D43 C45:C59 D46 C29:D31 C37 D21:D24 D36:D41 C5:C6">
+  <autoFilter ref="A1:C85"/>
+  <conditionalFormatting sqref="C40:C43 C62:C93 D70 C44:D44 C46:C60 D47 C29:D30 C38 D21:D24 D37:D42 C5:C6 C32:D32 D31">
+    <cfRule type="cellIs" dxfId="67" priority="75" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="76" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3102,23 +3144,23 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="63" priority="71" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="72" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
+  <conditionalFormatting sqref="C39">
+    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="66" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:D45">
     <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3126,7 +3168,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44:D44">
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3134,23 +3176,23 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C7 C14 C21:C24">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 D14">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C14 C21:C24">
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D14">
     <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3158,87 +3200,87 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C10">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D10">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C12">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D12">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C10">
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D10">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3246,7 +3288,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="C25:D28">
     <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3254,15 +3296,15 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:D28">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
-      <formula>"Oui"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
-      <formula>"Non"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>"Oui"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
     <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3270,7 +3312,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3278,7 +3320,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+  <conditionalFormatting sqref="C19:D20">
     <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3286,7 +3328,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:D20">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3294,7 +3336,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3302,7 +3344,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D15">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3310,7 +3352,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="C17:D17">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3318,7 +3360,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:D17">
+  <conditionalFormatting sqref="C18:D18">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3326,7 +3368,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:D18">
+  <conditionalFormatting sqref="C4">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3334,7 +3376,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
+  <conditionalFormatting sqref="C3:D3">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3342,7 +3384,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:D3">
+  <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3350,7 +3392,7 @@
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
+  <conditionalFormatting sqref="C31">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
@@ -3359,7 +3401,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:C84 C2:C45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C48:C85 C2:C46">
       <formula1>"Oui,Non"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>